<commit_message>
RDM-5122: Updated functional test cases.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
+++ b/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA80082-F3BD-FD40-9CE1-1C9DE7CA2CD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB41957C-8995-6248-9E03-7653447E5DE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="5400" windowWidth="28800" windowHeight="16520" tabRatio="823" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="823" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11227" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11231" uniqueCount="316">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1007,6 +1007,9 @@
   <si>
     <t>auto.test.cnp+localauth2@gmail.com</t>
   </si>
+  <si>
+    <t>auto.test.cnp+ctzn2@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -2597,7 +2600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2985,7 +2990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6660,10 +6667,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6883,7 +6890,7 @@
         <v>232</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>183</v>
@@ -6901,7 +6908,7 @@
         <v>232</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>183</v>
@@ -6919,9 +6926,27 @@
         <v>232</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="F15" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="72">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="73" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>183</v>
       </c>
     </row>
@@ -6939,6 +6964,7 @@
     <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-0D00-000009000000}"/>
     <hyperlink ref="C15" r:id="rId11" xr:uid="{00000000-0004-0000-0D00-00000A000000}"/>
     <hyperlink ref="C11" r:id="rId12" xr:uid="{26E3A81C-89F8-8F41-9E94-732455FAAB41}"/>
+    <hyperlink ref="C16" r:id="rId13" xr:uid="{FA6CB0C1-E3D4-8244-889B-E03B776FB7D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -6955,7 +6981,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7746,8 +7772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10420,8 +10446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="G313" sqref="G313"/>
+    <sheetView topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="H232" sqref="H232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15672,8 +15698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F795"/>
   <sheetViews>
-    <sheetView topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="G796" sqref="G796"/>
+    <sheetView topLeftCell="A737" workbookViewId="0">
+      <selection activeCell="H793" sqref="H793"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-5122: Fixed Citizen tests.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
+++ b/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB41957C-8995-6248-9E03-7653447E5DE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD0489E-2FCD-0246-BC5B-742E2F3FE507}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="823" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="823" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -999,9 +999,6 @@
     <t>caseworker-autotest1-panelmember</t>
   </si>
   <si>
-    <t>caseworker-autotest1-citizen</t>
-  </si>
-  <si>
     <t>auto.test.cnp+solc2@gmail.com</t>
   </si>
   <si>
@@ -1009,6 +1006,9 @@
   </si>
   <si>
     <t>auto.test.cnp+ctzn2@gmail.com</t>
+  </si>
+  <si>
+    <t>citizen-autotest1</t>
   </si>
 </sst>
 </file>
@@ -2990,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6669,8 +6669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6795,7 +6795,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>232</v>
@@ -6848,7 +6848,7 @@
         <v>42736</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>232</v>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="73" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>232</v>
@@ -6980,8 +6980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7289,7 +7289,7 @@
         <v>303</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>292</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7304,7 +7304,7 @@
         <v>303</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7319,7 +7319,7 @@
         <v>303</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>294</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7334,7 +7334,7 @@
         <v>303</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>295</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7349,7 +7349,7 @@
         <v>303</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>296</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7364,7 +7364,7 @@
         <v>303</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>297</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7379,7 +7379,7 @@
         <v>303</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>298</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7646,7 +7646,7 @@
         <v>276</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>292</v>
@@ -7661,7 +7661,7 @@
         <v>282</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>293</v>
@@ -7676,7 +7676,7 @@
         <v>283</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>294</v>
@@ -7691,7 +7691,7 @@
         <v>278</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>295</v>
@@ -7706,7 +7706,7 @@
         <v>279</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>296</v>
@@ -7721,7 +7721,7 @@
         <v>280</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>297</v>
@@ -7736,7 +7736,7 @@
         <v>281</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>298</v>
@@ -7751,7 +7751,7 @@
         <v>275</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>59</v>
@@ -7772,8 +7772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10010,8 +10010,8 @@
       <c r="D124" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E124" s="60" t="s">
-        <v>312</v>
+      <c r="E124" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F124" s="74" t="s">
         <v>59</v>
@@ -10028,8 +10028,8 @@
       <c r="D125" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E125" s="60" t="s">
-        <v>312</v>
+      <c r="E125" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F125" s="74" t="s">
         <v>59</v>
@@ -10046,8 +10046,8 @@
       <c r="D126" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E126" s="60" t="s">
-        <v>312</v>
+      <c r="E126" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F126" s="74" t="s">
         <v>59</v>
@@ -10064,8 +10064,8 @@
       <c r="D127" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E127" s="60" t="s">
-        <v>312</v>
+      <c r="E127" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F127" s="74" t="s">
         <v>59</v>
@@ -10082,8 +10082,8 @@
       <c r="D128" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E128" s="60" t="s">
-        <v>312</v>
+      <c r="E128" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F128" s="74" t="s">
         <v>59</v>
@@ -10100,8 +10100,8 @@
       <c r="D129" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E129" s="60" t="s">
-        <v>312</v>
+      <c r="E129" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F129" s="74" t="s">
         <v>59</v>
@@ -10118,8 +10118,8 @@
       <c r="D130" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E130" s="60" t="s">
-        <v>312</v>
+      <c r="E130" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F130" s="74" t="s">
         <v>59</v>
@@ -10136,8 +10136,8 @@
       <c r="D131" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E131" s="60" t="s">
-        <v>312</v>
+      <c r="E131" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F131" s="74" t="s">
         <v>59</v>
@@ -10154,8 +10154,8 @@
       <c r="D132" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E132" s="60" t="s">
-        <v>312</v>
+      <c r="E132" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F132" s="74" t="s">
         <v>59</v>
@@ -10172,8 +10172,8 @@
       <c r="D133" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E133" s="60" t="s">
-        <v>312</v>
+      <c r="E133" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F133" s="74" t="s">
         <v>59</v>
@@ -10190,8 +10190,8 @@
       <c r="D134" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E134" s="60" t="s">
-        <v>312</v>
+      <c r="E134" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F134" s="74" t="s">
         <v>59</v>
@@ -10208,8 +10208,8 @@
       <c r="D135" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E135" s="60" t="s">
-        <v>312</v>
+      <c r="E135" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F135" s="74" t="s">
         <v>59</v>
@@ -10226,8 +10226,8 @@
       <c r="D136" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E136" s="60" t="s">
-        <v>312</v>
+      <c r="E136" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F136" s="74" t="s">
         <v>59</v>
@@ -10244,8 +10244,8 @@
       <c r="D137" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E137" s="60" t="s">
-        <v>312</v>
+      <c r="E137" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F137" s="74" t="s">
         <v>59</v>
@@ -10262,8 +10262,8 @@
       <c r="D138" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E138" s="60" t="s">
-        <v>312</v>
+      <c r="E138" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F138" s="74" t="s">
         <v>59</v>
@@ -10280,8 +10280,8 @@
       <c r="D139" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E139" s="60" t="s">
-        <v>312</v>
+      <c r="E139" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F139" s="74" t="s">
         <v>59</v>
@@ -10298,8 +10298,8 @@
       <c r="D140" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E140" s="60" t="s">
-        <v>312</v>
+      <c r="E140" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F140" s="74" t="s">
         <v>59</v>
@@ -10316,8 +10316,8 @@
       <c r="D141" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E141" s="60" t="s">
-        <v>312</v>
+      <c r="E141" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F141" s="74" t="s">
         <v>59</v>
@@ -10334,8 +10334,8 @@
       <c r="D142" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E142" s="60" t="s">
-        <v>312</v>
+      <c r="E142" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F142" s="74" t="s">
         <v>59</v>
@@ -10352,8 +10352,8 @@
       <c r="D143" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E143" s="60" t="s">
-        <v>312</v>
+      <c r="E143" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F143" s="74" t="s">
         <v>59</v>
@@ -10370,8 +10370,8 @@
       <c r="D144" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E144" s="60" t="s">
-        <v>312</v>
+      <c r="E144" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F144" s="74" t="s">
         <v>59</v>
@@ -10388,8 +10388,8 @@
       <c r="D145" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="E145" s="60" t="s">
-        <v>312</v>
+      <c r="E145" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F145" s="74" t="s">
         <v>59</v>
@@ -10406,8 +10406,8 @@
       <c r="D146" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="E146" s="60" t="s">
-        <v>312</v>
+      <c r="E146" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F146" s="74" t="s">
         <v>59</v>
@@ -10424,8 +10424,8 @@
       <c r="D147" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="E147" s="60" t="s">
-        <v>312</v>
+      <c r="E147" s="24" t="s">
+        <v>315</v>
       </c>
       <c r="F147" s="74" t="s">
         <v>59</v>
@@ -10446,8 +10446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="H232" sqref="H232"/>
+    <sheetView topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="G247" sqref="G247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14831,7 +14831,7 @@
         <v>188</v>
       </c>
       <c r="E244" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F244" s="24" t="s">
         <v>59</v>
@@ -14849,7 +14849,7 @@
         <v>190</v>
       </c>
       <c r="E245" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F245" s="24" t="s">
         <v>59</v>
@@ -14867,7 +14867,7 @@
         <v>192</v>
       </c>
       <c r="E246" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F246" s="24" t="s">
         <v>59</v>
@@ -14885,7 +14885,7 @@
         <v>194</v>
       </c>
       <c r="E247" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F247" s="24" t="s">
         <v>59</v>
@@ -14903,7 +14903,7 @@
         <v>196</v>
       </c>
       <c r="E248" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F248" s="24" t="s">
         <v>59</v>
@@ -14921,7 +14921,7 @@
         <v>204</v>
       </c>
       <c r="E249" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F249" s="24" t="s">
         <v>59</v>
@@ -14939,7 +14939,7 @@
         <v>188</v>
       </c>
       <c r="E250" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F250" s="24" t="s">
         <v>59</v>
@@ -14957,7 +14957,7 @@
         <v>190</v>
       </c>
       <c r="E251" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F251" s="24" t="s">
         <v>59</v>
@@ -14975,7 +14975,7 @@
         <v>192</v>
       </c>
       <c r="E252" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F252" s="24" t="s">
         <v>59</v>
@@ -14993,7 +14993,7 @@
         <v>194</v>
       </c>
       <c r="E253" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F253" s="24" t="s">
         <v>59</v>
@@ -15011,7 +15011,7 @@
         <v>196</v>
       </c>
       <c r="E254" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F254" s="24" t="s">
         <v>59</v>
@@ -15029,7 +15029,7 @@
         <v>204</v>
       </c>
       <c r="E255" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F255" s="24" t="s">
         <v>59</v>
@@ -15047,7 +15047,7 @@
         <v>188</v>
       </c>
       <c r="E256" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F256" s="24" t="s">
         <v>59</v>
@@ -15065,7 +15065,7 @@
         <v>190</v>
       </c>
       <c r="E257" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F257" s="24" t="s">
         <v>59</v>
@@ -15083,7 +15083,7 @@
         <v>192</v>
       </c>
       <c r="E258" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F258" s="24" t="s">
         <v>59</v>
@@ -15101,7 +15101,7 @@
         <v>194</v>
       </c>
       <c r="E259" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F259" s="24" t="s">
         <v>59</v>
@@ -15119,7 +15119,7 @@
         <v>196</v>
       </c>
       <c r="E260" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F260" s="24" t="s">
         <v>59</v>
@@ -15137,7 +15137,7 @@
         <v>204</v>
       </c>
       <c r="E261" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F261" s="24" t="s">
         <v>59</v>
@@ -15155,7 +15155,7 @@
         <v>188</v>
       </c>
       <c r="E262" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F262" s="24" t="s">
         <v>59</v>
@@ -15173,7 +15173,7 @@
         <v>190</v>
       </c>
       <c r="E263" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F263" s="24" t="s">
         <v>59</v>
@@ -15191,7 +15191,7 @@
         <v>192</v>
       </c>
       <c r="E264" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F264" s="24" t="s">
         <v>59</v>
@@ -15209,7 +15209,7 @@
         <v>194</v>
       </c>
       <c r="E265" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F265" s="24" t="s">
         <v>59</v>
@@ -15227,7 +15227,7 @@
         <v>196</v>
       </c>
       <c r="E266" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F266" s="24" t="s">
         <v>59</v>
@@ -15245,7 +15245,7 @@
         <v>204</v>
       </c>
       <c r="E267" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F267" s="24" t="s">
         <v>59</v>
@@ -15263,7 +15263,7 @@
         <v>188</v>
       </c>
       <c r="E268" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F268" s="24" t="s">
         <v>59</v>
@@ -15281,7 +15281,7 @@
         <v>190</v>
       </c>
       <c r="E269" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F269" s="24" t="s">
         <v>59</v>
@@ -15299,7 +15299,7 @@
         <v>192</v>
       </c>
       <c r="E270" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F270" s="24" t="s">
         <v>59</v>
@@ -15317,7 +15317,7 @@
         <v>194</v>
       </c>
       <c r="E271" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F271" s="24" t="s">
         <v>59</v>
@@ -15335,7 +15335,7 @@
         <v>196</v>
       </c>
       <c r="E272" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F272" s="24" t="s">
         <v>59</v>
@@ -15353,7 +15353,7 @@
         <v>204</v>
       </c>
       <c r="E273" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F273" s="24" t="s">
         <v>59</v>
@@ -15371,7 +15371,7 @@
         <v>188</v>
       </c>
       <c r="E274" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F274" s="24" t="s">
         <v>59</v>
@@ -15389,7 +15389,7 @@
         <v>190</v>
       </c>
       <c r="E275" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F275" s="24" t="s">
         <v>59</v>
@@ -15407,7 +15407,7 @@
         <v>192</v>
       </c>
       <c r="E276" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F276" s="24" t="s">
         <v>59</v>
@@ -15425,7 +15425,7 @@
         <v>194</v>
       </c>
       <c r="E277" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F277" s="24" t="s">
         <v>59</v>
@@ -15443,7 +15443,7 @@
         <v>196</v>
       </c>
       <c r="E278" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F278" s="24" t="s">
         <v>59</v>
@@ -15461,7 +15461,7 @@
         <v>204</v>
       </c>
       <c r="E279" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F279" s="24" t="s">
         <v>59</v>
@@ -15479,7 +15479,7 @@
         <v>188</v>
       </c>
       <c r="E280" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F280" s="24" t="s">
         <v>59</v>
@@ -15497,7 +15497,7 @@
         <v>190</v>
       </c>
       <c r="E281" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F281" s="24" t="s">
         <v>59</v>
@@ -15515,7 +15515,7 @@
         <v>192</v>
       </c>
       <c r="E282" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F282" s="24" t="s">
         <v>59</v>
@@ -15533,7 +15533,7 @@
         <v>194</v>
       </c>
       <c r="E283" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F283" s="24" t="s">
         <v>59</v>
@@ -15551,7 +15551,7 @@
         <v>196</v>
       </c>
       <c r="E284" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F284" s="24" t="s">
         <v>59</v>
@@ -15569,7 +15569,7 @@
         <v>204</v>
       </c>
       <c r="E285" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F285" s="24" t="s">
         <v>59</v>
@@ -15587,7 +15587,7 @@
         <v>188</v>
       </c>
       <c r="E286" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F286" s="24" t="s">
         <v>59</v>
@@ -15605,7 +15605,7 @@
         <v>190</v>
       </c>
       <c r="E287" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F287" s="24" t="s">
         <v>59</v>
@@ -15623,7 +15623,7 @@
         <v>192</v>
       </c>
       <c r="E288" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F288" s="24" t="s">
         <v>59</v>
@@ -15641,7 +15641,7 @@
         <v>194</v>
       </c>
       <c r="E289" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F289" s="24" t="s">
         <v>59</v>
@@ -15659,7 +15659,7 @@
         <v>196</v>
       </c>
       <c r="E290" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F290" s="24" t="s">
         <v>59</v>
@@ -15677,7 +15677,7 @@
         <v>204</v>
       </c>
       <c r="E291" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F291" s="24" t="s">
         <v>59</v>
@@ -15698,8 +15698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F795"/>
   <sheetViews>
-    <sheetView topLeftCell="A737" workbookViewId="0">
-      <selection activeCell="H793" sqref="H793"/>
+    <sheetView topLeftCell="A771" workbookViewId="0">
+      <selection activeCell="G666" sqref="G666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27623,7 +27623,7 @@
         <v>133</v>
       </c>
       <c r="E664" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F664" s="24" t="s">
         <v>59</v>
@@ -27641,7 +27641,7 @@
         <v>135</v>
       </c>
       <c r="E665" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F665" s="24" t="s">
         <v>59</v>
@@ -27659,7 +27659,7 @@
         <v>137</v>
       </c>
       <c r="E666" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F666" s="24" t="s">
         <v>59</v>
@@ -27677,7 +27677,7 @@
         <v>142</v>
       </c>
       <c r="E667" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F667" s="24" t="s">
         <v>59</v>
@@ -27695,7 +27695,7 @@
         <v>144</v>
       </c>
       <c r="E668" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F668" s="24" t="s">
         <v>59</v>
@@ -27713,7 +27713,7 @@
         <v>148</v>
       </c>
       <c r="E669" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F669" s="24" t="s">
         <v>59</v>
@@ -27731,7 +27731,7 @@
         <v>156</v>
       </c>
       <c r="E670" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F670" s="24" t="s">
         <v>59</v>
@@ -27749,7 +27749,7 @@
         <v>244</v>
       </c>
       <c r="E671" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F671" s="24" t="s">
         <v>59</v>
@@ -27767,7 +27767,7 @@
         <v>154</v>
       </c>
       <c r="E672" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F672" s="24" t="s">
         <v>59</v>
@@ -27785,7 +27785,7 @@
         <v>158</v>
       </c>
       <c r="E673" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F673" s="24" t="s">
         <v>59</v>
@@ -27803,7 +27803,7 @@
         <v>168</v>
       </c>
       <c r="E674" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F674" s="24" t="s">
         <v>59</v>
@@ -27821,7 +27821,7 @@
         <v>240</v>
       </c>
       <c r="E675" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F675" s="24" t="s">
         <v>59</v>
@@ -27839,7 +27839,7 @@
         <v>237</v>
       </c>
       <c r="E676" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F676" s="24" t="s">
         <v>59</v>
@@ -27857,7 +27857,7 @@
         <v>223</v>
       </c>
       <c r="E677" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F677" s="24" t="s">
         <v>59</v>
@@ -27875,7 +27875,7 @@
         <v>252</v>
       </c>
       <c r="E678" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F678" s="24" t="s">
         <v>59</v>
@@ -27893,7 +27893,7 @@
         <v>263</v>
       </c>
       <c r="E679" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F679" s="24" t="s">
         <v>59</v>
@@ -27911,7 +27911,7 @@
         <v>133</v>
       </c>
       <c r="E680" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F680" s="24" t="s">
         <v>59</v>
@@ -27929,7 +27929,7 @@
         <v>135</v>
       </c>
       <c r="E681" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F681" s="24" t="s">
         <v>59</v>
@@ -27947,7 +27947,7 @@
         <v>137</v>
       </c>
       <c r="E682" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F682" s="24" t="s">
         <v>59</v>
@@ -27965,7 +27965,7 @@
         <v>142</v>
       </c>
       <c r="E683" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F683" s="24" t="s">
         <v>59</v>
@@ -27983,7 +27983,7 @@
         <v>144</v>
       </c>
       <c r="E684" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F684" s="24" t="s">
         <v>59</v>
@@ -28001,7 +28001,7 @@
         <v>148</v>
       </c>
       <c r="E685" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F685" s="24" t="s">
         <v>59</v>
@@ -28019,7 +28019,7 @@
         <v>156</v>
       </c>
       <c r="E686" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F686" s="24" t="s">
         <v>59</v>
@@ -28037,7 +28037,7 @@
         <v>244</v>
       </c>
       <c r="E687" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F687" s="24" t="s">
         <v>59</v>
@@ -28055,7 +28055,7 @@
         <v>154</v>
       </c>
       <c r="E688" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F688" s="24" t="s">
         <v>59</v>
@@ -28073,7 +28073,7 @@
         <v>158</v>
       </c>
       <c r="E689" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F689" s="24" t="s">
         <v>59</v>
@@ -28091,7 +28091,7 @@
         <v>168</v>
       </c>
       <c r="E690" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F690" s="24" t="s">
         <v>59</v>
@@ -28109,7 +28109,7 @@
         <v>240</v>
       </c>
       <c r="E691" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F691" s="24" t="s">
         <v>59</v>
@@ -28127,7 +28127,7 @@
         <v>237</v>
       </c>
       <c r="E692" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F692" s="24" t="s">
         <v>59</v>
@@ -28145,7 +28145,7 @@
         <v>223</v>
       </c>
       <c r="E693" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F693" s="24" t="s">
         <v>59</v>
@@ -28163,7 +28163,7 @@
         <v>248</v>
       </c>
       <c r="E694" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F694" s="24" t="s">
         <v>59</v>
@@ -28181,7 +28181,7 @@
         <v>252</v>
       </c>
       <c r="E695" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F695" s="24" t="s">
         <v>59</v>
@@ -28199,7 +28199,7 @@
         <v>263</v>
       </c>
       <c r="E696" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F696" s="24" t="s">
         <v>59</v>
@@ -28217,7 +28217,7 @@
         <v>133</v>
       </c>
       <c r="E697" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F697" s="24" t="s">
         <v>59</v>
@@ -28235,7 +28235,7 @@
         <v>135</v>
       </c>
       <c r="E698" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F698" s="24" t="s">
         <v>59</v>
@@ -28253,7 +28253,7 @@
         <v>137</v>
       </c>
       <c r="E699" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F699" s="24" t="s">
         <v>59</v>
@@ -28271,7 +28271,7 @@
         <v>142</v>
       </c>
       <c r="E700" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F700" s="24" t="s">
         <v>59</v>
@@ -28289,7 +28289,7 @@
         <v>144</v>
       </c>
       <c r="E701" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F701" s="24" t="s">
         <v>59</v>
@@ -28307,7 +28307,7 @@
         <v>148</v>
       </c>
       <c r="E702" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F702" s="24" t="s">
         <v>59</v>
@@ -28325,7 +28325,7 @@
         <v>156</v>
       </c>
       <c r="E703" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F703" s="24" t="s">
         <v>59</v>
@@ -28343,7 +28343,7 @@
         <v>244</v>
       </c>
       <c r="E704" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F704" s="24" t="s">
         <v>59</v>
@@ -28361,7 +28361,7 @@
         <v>154</v>
       </c>
       <c r="E705" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F705" s="24" t="s">
         <v>59</v>
@@ -28379,7 +28379,7 @@
         <v>158</v>
       </c>
       <c r="E706" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F706" s="24" t="s">
         <v>59</v>
@@ -28397,7 +28397,7 @@
         <v>168</v>
       </c>
       <c r="E707" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F707" s="24" t="s">
         <v>59</v>
@@ -28415,7 +28415,7 @@
         <v>240</v>
       </c>
       <c r="E708" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F708" s="24" t="s">
         <v>59</v>
@@ -28433,7 +28433,7 @@
         <v>237</v>
       </c>
       <c r="E709" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F709" s="24" t="s">
         <v>59</v>
@@ -28451,7 +28451,7 @@
         <v>223</v>
       </c>
       <c r="E710" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F710" s="24" t="s">
         <v>59</v>
@@ -28469,7 +28469,7 @@
         <v>252</v>
       </c>
       <c r="E711" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F711" s="24" t="s">
         <v>59</v>
@@ -28487,7 +28487,7 @@
         <v>263</v>
       </c>
       <c r="E712" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F712" s="24" t="s">
         <v>59</v>
@@ -28505,7 +28505,7 @@
         <v>133</v>
       </c>
       <c r="E713" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F713" s="24" t="s">
         <v>59</v>
@@ -28523,7 +28523,7 @@
         <v>135</v>
       </c>
       <c r="E714" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F714" s="24" t="s">
         <v>59</v>
@@ -28541,7 +28541,7 @@
         <v>137</v>
       </c>
       <c r="E715" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F715" s="24" t="s">
         <v>59</v>
@@ -28559,7 +28559,7 @@
         <v>142</v>
       </c>
       <c r="E716" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F716" s="24" t="s">
         <v>59</v>
@@ -28577,7 +28577,7 @@
         <v>144</v>
       </c>
       <c r="E717" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F717" s="24" t="s">
         <v>59</v>
@@ -28595,7 +28595,7 @@
         <v>148</v>
       </c>
       <c r="E718" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F718" s="24" t="s">
         <v>59</v>
@@ -28613,7 +28613,7 @@
         <v>156</v>
       </c>
       <c r="E719" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F719" s="24" t="s">
         <v>59</v>
@@ -28631,7 +28631,7 @@
         <v>244</v>
       </c>
       <c r="E720" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F720" s="24" t="s">
         <v>59</v>
@@ -28649,7 +28649,7 @@
         <v>154</v>
       </c>
       <c r="E721" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F721" s="24" t="s">
         <v>59</v>
@@ -28667,7 +28667,7 @@
         <v>158</v>
       </c>
       <c r="E722" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F722" s="24" t="s">
         <v>59</v>
@@ -28685,7 +28685,7 @@
         <v>168</v>
       </c>
       <c r="E723" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F723" s="24" t="s">
         <v>59</v>
@@ -28703,7 +28703,7 @@
         <v>240</v>
       </c>
       <c r="E724" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F724" s="24" t="s">
         <v>59</v>
@@ -28721,7 +28721,7 @@
         <v>237</v>
       </c>
       <c r="E725" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F725" s="24" t="s">
         <v>59</v>
@@ -28739,7 +28739,7 @@
         <v>223</v>
       </c>
       <c r="E726" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F726" s="24" t="s">
         <v>59</v>
@@ -28757,7 +28757,7 @@
         <v>248</v>
       </c>
       <c r="E727" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F727" s="24" t="s">
         <v>59</v>
@@ -28775,7 +28775,7 @@
         <v>252</v>
       </c>
       <c r="E728" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F728" s="24" t="s">
         <v>59</v>
@@ -28793,7 +28793,7 @@
         <v>263</v>
       </c>
       <c r="E729" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F729" s="24" t="s">
         <v>59</v>
@@ -28811,7 +28811,7 @@
         <v>133</v>
       </c>
       <c r="E730" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F730" s="24" t="s">
         <v>59</v>
@@ -28829,7 +28829,7 @@
         <v>135</v>
       </c>
       <c r="E731" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F731" s="24" t="s">
         <v>59</v>
@@ -28847,7 +28847,7 @@
         <v>137</v>
       </c>
       <c r="E732" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F732" s="24" t="s">
         <v>59</v>
@@ -28865,7 +28865,7 @@
         <v>142</v>
       </c>
       <c r="E733" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F733" s="24" t="s">
         <v>59</v>
@@ -28883,7 +28883,7 @@
         <v>144</v>
       </c>
       <c r="E734" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F734" s="24" t="s">
         <v>59</v>
@@ -28901,7 +28901,7 @@
         <v>148</v>
       </c>
       <c r="E735" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F735" s="24" t="s">
         <v>59</v>
@@ -28919,7 +28919,7 @@
         <v>156</v>
       </c>
       <c r="E736" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F736" s="24" t="s">
         <v>59</v>
@@ -28937,7 +28937,7 @@
         <v>244</v>
       </c>
       <c r="E737" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F737" s="24" t="s">
         <v>59</v>
@@ -28955,7 +28955,7 @@
         <v>154</v>
       </c>
       <c r="E738" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F738" s="24" t="s">
         <v>59</v>
@@ -28973,7 +28973,7 @@
         <v>158</v>
       </c>
       <c r="E739" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F739" s="24" t="s">
         <v>59</v>
@@ -28991,7 +28991,7 @@
         <v>168</v>
       </c>
       <c r="E740" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F740" s="24" t="s">
         <v>59</v>
@@ -29009,7 +29009,7 @@
         <v>240</v>
       </c>
       <c r="E741" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F741" s="24" t="s">
         <v>59</v>
@@ -29027,7 +29027,7 @@
         <v>237</v>
       </c>
       <c r="E742" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F742" s="24" t="s">
         <v>59</v>
@@ -29045,7 +29045,7 @@
         <v>223</v>
       </c>
       <c r="E743" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F743" s="24" t="s">
         <v>59</v>
@@ -29063,7 +29063,7 @@
         <v>252</v>
       </c>
       <c r="E744" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F744" s="24" t="s">
         <v>59</v>
@@ -29081,7 +29081,7 @@
         <v>263</v>
       </c>
       <c r="E745" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F745" s="24" t="s">
         <v>59</v>
@@ -29099,7 +29099,7 @@
         <v>133</v>
       </c>
       <c r="E746" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F746" s="24" t="s">
         <v>59</v>
@@ -29117,7 +29117,7 @@
         <v>135</v>
       </c>
       <c r="E747" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F747" s="24" t="s">
         <v>59</v>
@@ -29135,7 +29135,7 @@
         <v>137</v>
       </c>
       <c r="E748" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F748" s="24" t="s">
         <v>59</v>
@@ -29153,7 +29153,7 @@
         <v>142</v>
       </c>
       <c r="E749" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F749" s="24" t="s">
         <v>59</v>
@@ -29171,7 +29171,7 @@
         <v>144</v>
       </c>
       <c r="E750" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F750" s="24" t="s">
         <v>59</v>
@@ -29189,7 +29189,7 @@
         <v>148</v>
       </c>
       <c r="E751" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F751" s="24" t="s">
         <v>59</v>
@@ -29207,7 +29207,7 @@
         <v>156</v>
       </c>
       <c r="E752" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F752" s="24" t="s">
         <v>59</v>
@@ -29225,7 +29225,7 @@
         <v>244</v>
       </c>
       <c r="E753" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F753" s="24" t="s">
         <v>59</v>
@@ -29243,7 +29243,7 @@
         <v>154</v>
       </c>
       <c r="E754" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F754" s="24" t="s">
         <v>59</v>
@@ -29261,7 +29261,7 @@
         <v>158</v>
       </c>
       <c r="E755" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F755" s="24" t="s">
         <v>59</v>
@@ -29279,7 +29279,7 @@
         <v>168</v>
       </c>
       <c r="E756" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F756" s="24" t="s">
         <v>59</v>
@@ -29297,7 +29297,7 @@
         <v>240</v>
       </c>
       <c r="E757" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F757" s="24" t="s">
         <v>59</v>
@@ -29315,7 +29315,7 @@
         <v>237</v>
       </c>
       <c r="E758" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F758" s="24" t="s">
         <v>59</v>
@@ -29333,7 +29333,7 @@
         <v>223</v>
       </c>
       <c r="E759" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F759" s="24" t="s">
         <v>59</v>
@@ -29351,7 +29351,7 @@
         <v>248</v>
       </c>
       <c r="E760" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F760" s="24" t="s">
         <v>59</v>
@@ -29369,7 +29369,7 @@
         <v>252</v>
       </c>
       <c r="E761" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F761" s="24" t="s">
         <v>59</v>
@@ -29387,7 +29387,7 @@
         <v>263</v>
       </c>
       <c r="E762" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F762" s="24" t="s">
         <v>59</v>
@@ -29405,7 +29405,7 @@
         <v>133</v>
       </c>
       <c r="E763" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F763" s="24" t="s">
         <v>59</v>
@@ -29423,7 +29423,7 @@
         <v>135</v>
       </c>
       <c r="E764" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F764" s="24" t="s">
         <v>59</v>
@@ -29441,7 +29441,7 @@
         <v>137</v>
       </c>
       <c r="E765" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F765" s="24" t="s">
         <v>59</v>
@@ -29459,7 +29459,7 @@
         <v>142</v>
       </c>
       <c r="E766" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F766" s="24" t="s">
         <v>59</v>
@@ -29477,7 +29477,7 @@
         <v>144</v>
       </c>
       <c r="E767" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F767" s="24" t="s">
         <v>59</v>
@@ -29495,7 +29495,7 @@
         <v>148</v>
       </c>
       <c r="E768" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F768" s="24" t="s">
         <v>59</v>
@@ -29513,7 +29513,7 @@
         <v>156</v>
       </c>
       <c r="E769" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F769" s="24" t="s">
         <v>59</v>
@@ -29531,7 +29531,7 @@
         <v>244</v>
       </c>
       <c r="E770" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F770" s="24" t="s">
         <v>59</v>
@@ -29549,7 +29549,7 @@
         <v>154</v>
       </c>
       <c r="E771" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F771" s="24" t="s">
         <v>59</v>
@@ -29567,7 +29567,7 @@
         <v>158</v>
       </c>
       <c r="E772" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F772" s="24" t="s">
         <v>59</v>
@@ -29585,7 +29585,7 @@
         <v>168</v>
       </c>
       <c r="E773" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F773" s="24" t="s">
         <v>59</v>
@@ -29603,7 +29603,7 @@
         <v>240</v>
       </c>
       <c r="E774" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F774" s="24" t="s">
         <v>59</v>
@@ -29621,7 +29621,7 @@
         <v>237</v>
       </c>
       <c r="E775" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F775" s="24" t="s">
         <v>59</v>
@@ -29639,7 +29639,7 @@
         <v>223</v>
       </c>
       <c r="E776" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F776" s="24" t="s">
         <v>59</v>
@@ -29657,7 +29657,7 @@
         <v>252</v>
       </c>
       <c r="E777" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F777" s="24" t="s">
         <v>59</v>
@@ -29675,7 +29675,7 @@
         <v>263</v>
       </c>
       <c r="E778" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F778" s="24" t="s">
         <v>59</v>
@@ -29693,7 +29693,7 @@
         <v>133</v>
       </c>
       <c r="E779" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F779" s="24" t="s">
         <v>59</v>
@@ -29711,7 +29711,7 @@
         <v>135</v>
       </c>
       <c r="E780" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F780" s="24" t="s">
         <v>59</v>
@@ -29729,7 +29729,7 @@
         <v>137</v>
       </c>
       <c r="E781" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F781" s="24" t="s">
         <v>59</v>
@@ -29747,7 +29747,7 @@
         <v>142</v>
       </c>
       <c r="E782" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F782" s="24" t="s">
         <v>59</v>
@@ -29765,7 +29765,7 @@
         <v>144</v>
       </c>
       <c r="E783" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F783" s="24" t="s">
         <v>59</v>
@@ -29783,7 +29783,7 @@
         <v>148</v>
       </c>
       <c r="E784" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F784" s="24" t="s">
         <v>59</v>
@@ -29801,7 +29801,7 @@
         <v>156</v>
       </c>
       <c r="E785" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F785" s="24" t="s">
         <v>59</v>
@@ -29819,7 +29819,7 @@
         <v>244</v>
       </c>
       <c r="E786" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F786" s="24" t="s">
         <v>59</v>
@@ -29837,7 +29837,7 @@
         <v>154</v>
       </c>
       <c r="E787" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F787" s="24" t="s">
         <v>59</v>
@@ -29855,7 +29855,7 @@
         <v>158</v>
       </c>
       <c r="E788" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F788" s="24" t="s">
         <v>59</v>
@@ -29873,7 +29873,7 @@
         <v>168</v>
       </c>
       <c r="E789" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F789" s="24" t="s">
         <v>59</v>
@@ -29891,7 +29891,7 @@
         <v>240</v>
       </c>
       <c r="E790" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F790" s="24" t="s">
         <v>59</v>
@@ -29909,7 +29909,7 @@
         <v>237</v>
       </c>
       <c r="E791" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F791" s="24" t="s">
         <v>59</v>
@@ -29927,7 +29927,7 @@
         <v>223</v>
       </c>
       <c r="E792" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F792" s="24" t="s">
         <v>59</v>
@@ -29945,7 +29945,7 @@
         <v>248</v>
       </c>
       <c r="E793" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F793" s="24" t="s">
         <v>59</v>
@@ -29963,7 +29963,7 @@
         <v>252</v>
       </c>
       <c r="E794" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F794" s="24" t="s">
         <v>59</v>
@@ -29981,7 +29981,7 @@
         <v>263</v>
       </c>
       <c r="E795" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F795" s="24" t="s">
         <v>59</v>
@@ -30002,7 +30002,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0"/>
+    <sheetView topLeftCell="C73" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H148" sqref="H148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -30011,7 +30013,7 @@
     <col min="3" max="3" width="25.5" style="81" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="81" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.6640625" style="81" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="81" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" style="81" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="81"/>
   </cols>
@@ -32489,7 +32491,7 @@
         <v>213</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G124" s="81" t="s">
         <v>59</v>
@@ -32509,7 +32511,7 @@
         <v>215</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G125" s="81" t="s">
         <v>59</v>
@@ -32529,7 +32531,7 @@
         <v>221</v>
       </c>
       <c r="F126" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G126" s="81" t="s">
         <v>59</v>
@@ -32549,7 +32551,7 @@
         <v>213</v>
       </c>
       <c r="F127" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G127" s="81" t="s">
         <v>59</v>
@@ -32569,7 +32571,7 @@
         <v>215</v>
       </c>
       <c r="F128" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G128" s="81" t="s">
         <v>59</v>
@@ -32589,7 +32591,7 @@
         <v>221</v>
       </c>
       <c r="F129" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G129" s="81" t="s">
         <v>59</v>
@@ -32609,7 +32611,7 @@
         <v>213</v>
       </c>
       <c r="F130" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G130" s="81" t="s">
         <v>59</v>
@@ -32629,7 +32631,7 @@
         <v>215</v>
       </c>
       <c r="F131" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G131" s="81" t="s">
         <v>59</v>
@@ -32649,7 +32651,7 @@
         <v>221</v>
       </c>
       <c r="F132" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G132" s="81" t="s">
         <v>59</v>
@@ -32669,7 +32671,7 @@
         <v>213</v>
       </c>
       <c r="F133" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G133" s="81" t="s">
         <v>59</v>
@@ -32689,7 +32691,7 @@
         <v>215</v>
       </c>
       <c r="F134" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G134" s="81" t="s">
         <v>59</v>
@@ -32709,7 +32711,7 @@
         <v>221</v>
       </c>
       <c r="F135" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G135" s="81" t="s">
         <v>59</v>
@@ -32729,7 +32731,7 @@
         <v>213</v>
       </c>
       <c r="F136" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G136" s="81" t="s">
         <v>59</v>
@@ -32749,7 +32751,7 @@
         <v>215</v>
       </c>
       <c r="F137" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G137" s="81" t="s">
         <v>59</v>
@@ -32769,7 +32771,7 @@
         <v>221</v>
       </c>
       <c r="F138" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G138" s="81" t="s">
         <v>59</v>
@@ -32789,7 +32791,7 @@
         <v>213</v>
       </c>
       <c r="F139" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G139" s="81" t="s">
         <v>59</v>
@@ -32809,7 +32811,7 @@
         <v>215</v>
       </c>
       <c r="F140" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G140" s="81" t="s">
         <v>59</v>
@@ -32829,7 +32831,7 @@
         <v>221</v>
       </c>
       <c r="F141" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G141" s="81" t="s">
         <v>59</v>
@@ -32849,7 +32851,7 @@
         <v>213</v>
       </c>
       <c r="F142" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G142" s="81" t="s">
         <v>59</v>
@@ -32869,7 +32871,7 @@
         <v>215</v>
       </c>
       <c r="F143" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G143" s="81" t="s">
         <v>59</v>
@@ -32889,7 +32891,7 @@
         <v>221</v>
       </c>
       <c r="F144" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G144" s="81" t="s">
         <v>59</v>
@@ -32909,7 +32911,7 @@
         <v>213</v>
       </c>
       <c r="F145" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G145" s="81" t="s">
         <v>59</v>
@@ -32929,7 +32931,7 @@
         <v>215</v>
       </c>
       <c r="F146" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G146" s="81" t="s">
         <v>59</v>
@@ -32949,7 +32951,7 @@
         <v>221</v>
       </c>
       <c r="F147" s="24" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G147" s="81" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
RDM-5122: Updates: 1. For AAT_AUTH_4, set the permissions to CRUD initially and then reduce to "U" only. 2. Introduced a Timeunit.SECONDS.sleep() after new definition upload.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
+++ b/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD0489E-2FCD-0246-BC5B-742E2F3FE507}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B592A-5FAD-A645-B8F7-5EDB2C5C0331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="823" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="823" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -6980,8 +6980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7574,7 +7574,7 @@
         <v>311</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>295</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
case definition import with 30 second timeout
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
+++ b/src/aat/resources/CCD_CNP_RDM5118_5122_Extended.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/664355/Documents/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B592A-5FAD-A645-B8F7-5EDB2C5C0331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D435835A-72E9-584D-9977-BEF669A8F6F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="823" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="15840" windowHeight="19220" tabRatio="823" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -2990,7 +2990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
@@ -6670,7 +6670,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6980,8 +6980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7574,7 +7574,7 @@
         <v>311</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>59</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -10446,7 +10446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G247" sqref="G247"/>
     </sheetView>
   </sheetViews>
@@ -15698,8 +15698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F795"/>
   <sheetViews>
-    <sheetView topLeftCell="A771" workbookViewId="0">
-      <selection activeCell="G666" sqref="G666"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32967,7 +32967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>